<commit_message>
added all bash scripts to construct database
</commit_message>
<xml_diff>
--- a/wind_database_metadata.xlsx
+++ b/wind_database_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spann\Documents\Research\reynolds_scales_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126A9F20-BBC6-4C13-B13E-AE6EE1D9E04A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DCC0BDE-120A-4B81-A300-BDE53A63FC97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{60C75D1D-90E2-4A5F-AB16-E1D6DF71A971}"/>
+    <workbookView xWindow="-25320" yWindow="-2025" windowWidth="25440" windowHeight="15990" xr2:uid="{60C75D1D-90E2-4A5F-AB16-E1D6DF71A971}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="129">
   <si>
     <t>Variables for Wind database</t>
   </si>
@@ -254,9 +254,6 @@
     <t>Dataset OR derivation method</t>
   </si>
   <si>
-    <t>From NRL formulary</t>
-  </si>
-  <si>
     <t>7.43e-3*(Te**1/2)(ne**-1/2)</t>
   </si>
   <si>
@@ -344,15 +341,9 @@
     <t>Also available from OMNI: proton_density</t>
   </si>
   <si>
-    <t>Debye length</t>
-  </si>
-  <si>
     <t>ld</t>
   </si>
   <si>
-    <t>2 wk average</t>
-  </si>
-  <si>
     <t xml:space="preserve">np.sqrt((Bx-mean(Bx))**2+(By-mean(By))**2+(Bz-mean(Bz))**2) </t>
   </si>
   <si>
@@ -365,24 +356,6 @@
     <t>Bwind</t>
   </si>
   <si>
-    <t>Calculated from high-res Wind data, with mean calculated from entire dataset</t>
-  </si>
-  <si>
-    <t>(2.38e-5)*(Te**1/2)*(Bomni**-1)</t>
-  </si>
-  <si>
-    <t>(1.02e-3)*(Ti**1/2)*(Bomni**-1)</t>
-  </si>
-  <si>
-    <t>(4.03e-16)*ne*Te*(Bomni**-2)</t>
-  </si>
-  <si>
-    <t>(4.03e-16)*ni*Ti*(Bomni**-2)</t>
-  </si>
-  <si>
-    <t>(2.18e6)*(ni**-1/2)*Bomni</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -408,6 +381,48 @@
   </si>
   <si>
     <t>Numerical variable</t>
+  </si>
+  <si>
+    <t>From NRL formulary (converting cm to km and nT to Gauss)</t>
+  </si>
+  <si>
+    <t>Calculated from high-res Wind data, with mean calculated from entire dataset. Typically then divide by B0 (sqrt of sum of squared mean components) to get variable of interest</t>
+  </si>
+  <si>
+    <t>1 wk average</t>
+  </si>
+  <si>
+    <t>Debye length (electron)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From NRL formulary (converting cm to km and nT to Gauss). </t>
+  </si>
+  <si>
+    <t>Found to be 0.4Hz by Wang2017. Found ratio fb/fdi to be 0.48+-0.06</t>
+  </si>
+  <si>
+    <t>Wang2017 used 0.005-0.2Hz</t>
+  </si>
+  <si>
+    <t>Wang2017 used 0.5-1.4Hz</t>
+  </si>
+  <si>
+    <t>From NRL formulary (converting cm to km and nT to Gauss). Wang2017: ranged from 0.1 to 1.3</t>
+  </si>
+  <si>
+    <t>(2.38e-5)*(Te**1/2)*((Bomni*e-5)**-1)</t>
+  </si>
+  <si>
+    <t>(1.02e-3)*(Ti**1/2)*((Bomni*e-5)**-1)</t>
+  </si>
+  <si>
+    <t>(4.03e-16)*ne*Te*((Bomni*e-5)**-2)</t>
+  </si>
+  <si>
+    <t>(4.03e-16)*ni*Ti*((Bomni*e-5)**-2)</t>
+  </si>
+  <si>
+    <t>(2.18e6)*(ni**-1/2)*(Bomni*e-5)</t>
   </si>
 </sst>
 </file>
@@ -630,7 +645,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -668,12 +683,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -690,6 +699,14 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
@@ -698,6 +715,62 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -720,62 +793,6 @@
           <color indexed="64"/>
         </left>
         <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -947,10 +964,10 @@
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{69A8CBD7-495C-4F77-9807-78FEB8E3AF0F}" name="Name in database" dataDxfId="5" dataCellStyle="Normal"/>
     <tableColumn id="2" xr3:uid="{D6A57239-58B9-4C96-93D7-C08DD9CBA495}" name="Full name" dataDxfId="4" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{E29AF60E-8C37-476C-9021-82D4040D9DF6}" name="2 wk average" dataDxfId="0" dataCellStyle="40% - Accent3"/>
-    <tableColumn id="3" xr3:uid="{A5AF20BE-333B-48B4-AC25-68960254473D}" name="Unit" dataDxfId="3" dataCellStyle="40% - Accent3"/>
-    <tableColumn id="6" xr3:uid="{6FEA0C9A-F1C6-4A66-9476-C4AE4F69ED82}" name="Dataset OR derivation method" dataDxfId="2" dataCellStyle="40% - Accent3"/>
-    <tableColumn id="8" xr3:uid="{7BBB7C73-A571-43CF-A5A8-5DD1CD903E7D}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{E29AF60E-8C37-476C-9021-82D4040D9DF6}" name="1 wk average" dataDxfId="3" dataCellStyle="40% - Accent3"/>
+    <tableColumn id="3" xr3:uid="{A5AF20BE-333B-48B4-AC25-68960254473D}" name="Unit" dataDxfId="2" dataCellStyle="40% - Accent3"/>
+    <tableColumn id="6" xr3:uid="{6FEA0C9A-F1C6-4A66-9476-C4AE4F69ED82}" name="Dataset OR derivation method" dataDxfId="1" dataCellStyle="40% - Accent3"/>
+    <tableColumn id="8" xr3:uid="{7BBB7C73-A571-43CF-A5A8-5DD1CD903E7D}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1256,10 +1273,10 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="8" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomRight" activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1274,22 +1291,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="22"/>
@@ -1299,27 +1316,27 @@
       <c r="E3" s="22"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="44" t="s">
-        <v>84</v>
+      <c r="A4" s="42" t="s">
+        <v>83</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
-        <v>122</v>
+      <c r="A5" s="43" t="s">
+        <v>113</v>
       </c>
       <c r="B5" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="46" t="s">
-        <v>123</v>
+      <c r="A6" s="44" t="s">
+        <v>114</v>
       </c>
       <c r="B6" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1330,7 +1347,7 @@
         <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>21</v>
@@ -1343,101 +1360,101 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="43" t="s">
-        <v>74</v>
+      <c r="A9" s="41" t="s">
+        <v>73</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="D9" s="20" t="s">
         <v>45</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="43" t="s">
-        <v>75</v>
+      <c r="A10" s="41" t="s">
+        <v>74</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>45</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="43" t="s">
-        <v>76</v>
+      <c r="A11" s="41" t="s">
+        <v>75</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>45</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C12" s="34">
-        <v>6.3</v>
+        <v>6.8</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="F12" s="37"/>
+        <v>95</v>
+      </c>
+      <c r="F12" s="35"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="B13" s="39" t="s">
-        <v>95</v>
-      </c>
-      <c r="C13" s="41">
-        <v>6.6</v>
-      </c>
-      <c r="D13" s="40" t="s">
+      <c r="A13" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="39">
+        <v>6.5</v>
+      </c>
+      <c r="D13" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="40" t="s">
-        <v>107</v>
-      </c>
-      <c r="F13" s="41" t="s">
-        <v>120</v>
+      <c r="E13" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="F13" s="39" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1448,7 +1465,7 @@
         <v>37</v>
       </c>
       <c r="C14" s="6">
-        <v>2.4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>41</v>
@@ -1457,7 +1474,7 @@
         <v>70</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1468,7 +1485,7 @@
         <v>20</v>
       </c>
       <c r="C15" s="6">
-        <v>415</v>
+        <v>427</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>23</v>
@@ -1477,7 +1494,7 @@
         <v>67</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1488,13 +1505,13 @@
         <v>65</v>
       </c>
       <c r="C16" s="32">
-        <v>3.5</v>
+        <v>3.9</v>
       </c>
       <c r="D16" s="29" t="s">
         <v>25</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F16" s="29"/>
     </row>
@@ -1506,10 +1523,10 @@
         <v>29</v>
       </c>
       <c r="C17" s="32">
-        <v>14</v>
+        <v>13.5</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E17" s="29" t="s">
         <v>69</v>
@@ -1524,7 +1541,7 @@
         <v>24</v>
       </c>
       <c r="C18" s="32">
-        <v>4.3</v>
+        <v>4.8</v>
       </c>
       <c r="D18" s="29" t="s">
         <v>25</v>
@@ -1533,7 +1550,7 @@
         <v>68</v>
       </c>
       <c r="F18" s="29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1544,13 +1561,13 @@
         <v>28</v>
       </c>
       <c r="C19" s="32">
-        <v>20</v>
+        <v>17.3</v>
       </c>
       <c r="D19" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="E19" s="29" t="s">
         <v>98</v>
-      </c>
-      <c r="E19" s="29" t="s">
-        <v>99</v>
       </c>
       <c r="F19" s="29"/>
     </row>
@@ -1561,17 +1578,17 @@
       <c r="B20" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="42">
-        <v>1.5E-5</v>
+      <c r="C20" s="47">
+        <v>1.39</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>72</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1581,17 +1598,17 @@
       <c r="B21" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="42">
-        <v>7.2999999999999996E-4</v>
+      <c r="C21" s="48">
+        <v>68</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>72</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1602,16 +1619,16 @@
         <v>31</v>
       </c>
       <c r="C22" s="12">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>43</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>72</v>
+        <v>92</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1622,16 +1639,16 @@
         <v>30</v>
       </c>
       <c r="C23" s="9">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1641,17 +1658,17 @@
       <c r="B24" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="9">
-        <v>5.5</v>
+      <c r="C24" s="40">
+        <v>5.2000000000000002E-6</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>72</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1661,17 +1678,17 @@
       <c r="B25" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="9">
-        <v>8.5</v>
+      <c r="C25" s="40">
+        <v>8.4999999999999999E-6</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>72</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1681,25 +1698,25 @@
       <c r="B26" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="42">
-        <v>7300000</v>
+      <c r="C26" s="48">
+        <v>74</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>72</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="C27" s="9">
         <v>1.6E-2</v>
@@ -1708,10 +1725,10 @@
         <v>43</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>72</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1728,10 +1745,10 @@
         <v>45</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1750,7 +1767,9 @@
       <c r="E29" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="F29" s="15"/>
+      <c r="F29" s="15" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
@@ -1768,7 +1787,9 @@
       <c r="E30" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F30" s="15"/>
+      <c r="F30" s="15" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
@@ -1786,14 +1807,16 @@
       <c r="E31" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F31" s="15"/>
+      <c r="F31" s="15" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>13</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C32" s="15">
         <v>1710</v>
@@ -1802,7 +1825,7 @@
         <v>27</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F32" s="15"/>
     </row>
@@ -1811,7 +1834,7 @@
         <v>14</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C33" s="15">
         <v>1664</v>
@@ -1820,7 +1843,7 @@
         <v>27</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F33" s="15"/>
     </row>
@@ -1829,7 +1852,7 @@
         <v>15</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C34" s="15">
         <v>1739</v>
@@ -1838,7 +1861,7 @@
         <v>27</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F34" s="15"/>
     </row>
@@ -1928,10 +1951,10 @@
         <v>27</v>
       </c>
       <c r="E39" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="F39" s="18" t="s">
         <v>91</v>
-      </c>
-      <c r="F39" s="18" t="s">
-        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating readme, text output
</commit_message>
<xml_diff>
--- a/wind_database_metadata.xlsx
+++ b/wind_database_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spann\Documents\Research\reynolds_scales_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7511C88-D6EB-4897-833D-E617CF90DCAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02A4D57-3AFF-459A-8090-29DF55E1AFC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-2025" windowWidth="25440" windowHeight="15990" xr2:uid="{60C75D1D-90E2-4A5F-AB16-E1D6DF71A971}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{60C75D1D-90E2-4A5F-AB16-E1D6DF71A971}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="130">
   <si>
     <t>Variables for Wind database</t>
   </si>
@@ -423,6 +423,9 @@
   </si>
   <si>
     <t>(7.43e-3)*(Te**1/2)(ne**-1/2)</t>
+  </si>
+  <si>
+    <t>"+ energy (acov at 0 lag), c.f. Mark's values"</t>
   </si>
 </sst>
 </file>
@@ -651,7 +654,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -706,13 +709,14 @@
     </xf>
     <xf numFmtId="2" fontId="2" fillId="3" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="3" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="6" borderId="6" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="6" borderId="6" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
@@ -1276,13 +1280,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{993E126D-618E-4F8A-9C35-3E793C167672}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="8" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1297,22 +1301,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="22"/>
@@ -1664,7 +1668,7 @@
       <c r="B24" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="48">
+      <c r="C24" s="46">
         <v>0.52</v>
       </c>
       <c r="D24" s="8" t="s">
@@ -1684,7 +1688,7 @@
       <c r="B25" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="48">
+      <c r="C25" s="46">
         <v>0.85</v>
       </c>
       <c r="D25" s="8" t="s">
@@ -1961,6 +1965,11 @@
       </c>
       <c r="F39" s="18" t="s">
         <v>90</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="49" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commiting final data files to parent repo
</commit_message>
<xml_diff>
--- a/wind_database_metadata.xlsx
+++ b/wind_database_metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spann\Documents\Research\Code repos\reynolds_scales_project\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spann\Documents\Research\Code repos\reynolds_scales_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349236E3-98A3-4C21-B2E6-F7129A0CDCF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0FD329-7DED-45BF-8229-F6FF37FF6062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{60C75D1D-90E2-4A5F-AB16-E1D6DF71A971}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="10455" windowHeight="10905" xr2:uid="{60C75D1D-90E2-4A5F-AB16-E1D6DF71A971}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1378,11 +1378,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{993E126D-618E-4F8A-9C35-3E793C167672}">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="F24" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="1" ySplit="8" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
+      <selection pane="bottomRight" activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2137,7 +2137,7 @@
       <c r="E43" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="F43" s="40"/>
+      <c r="F43" s="16"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="43" t="s">
@@ -2153,7 +2153,7 @@
       <c r="E44" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="F44" s="40"/>
+      <c r="F44" s="16"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="43" t="s">
@@ -2169,7 +2169,7 @@
       <c r="E45" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="F45" s="40"/>
+      <c r="F45" s="16"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="43" t="s">
@@ -2185,7 +2185,7 @@
       <c r="E46" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="F46" s="40"/>
+      <c r="F46" s="16"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="43" t="s">
@@ -2201,7 +2201,7 @@
       <c r="E47" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="F47" s="40"/>
+      <c r="F47" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
filling in missing values in metadata file
</commit_message>
<xml_diff>
--- a/wind_database_metadata.xlsx
+++ b/wind_database_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spann\Documents\Research\Code repos\reynolds_scales_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0FD329-7DED-45BF-8229-F6FF37FF6062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A0E12E-2B94-4789-9D13-1DC66099B546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="10455" windowHeight="10905" xr2:uid="{60C75D1D-90E2-4A5F-AB16-E1D6DF71A971}"/>
+    <workbookView xWindow="10140" yWindow="0" windowWidth="10455" windowHeight="11625" xr2:uid="{60C75D1D-90E2-4A5F-AB16-E1D6DF71A971}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -443,12 +443,6 @@
     <t>Variables taken directly from CDF files from SPDF. Missing values are linearly interpolated, unless comprising &gt;10% of the interval, in which case the entire interval is set to missing</t>
   </si>
   <si>
-    <t xml:space="preserve">Observations show to be about -8/3 (-2.67). Wang2017 used a range of 0.5-1.4Hz. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Theory tells us should be -5/3 (1.67). Wang2017 used a range of 0.005-0.2Hz. </t>
-  </si>
-  <si>
     <t>Power-law fit to power spectrum over range 0.005&lt; f &lt; 0.2</t>
   </si>
   <si>
@@ -525,6 +519,38 @@
   </si>
   <si>
     <t>Should be around 0.4-0.5Hz (Weygand2007), corresponding to distances of 600-1000km. Any statistical analysis should refer to Vech2018</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Observations show to be about -8/3 (-2.67). Wang2017 used a range of 0.5-1.4Hz. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Expected to be correlated with temperature (Leamon1998)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Theory tells us should be -5/3 (1.67). Wang2017 used a range of 0.005-0.2Hz. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Expected to be correlated with temperature (Leamon1998)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -751,7 +777,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -813,6 +839,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="3" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
@@ -1378,11 +1406,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{993E126D-618E-4F8A-9C35-3E793C167672}">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="1" ySplit="8" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="E50" sqref="E50"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1809,7 +1837,7 @@
         <v>22</v>
       </c>
       <c r="C26" s="38">
-        <v>111.8</v>
+        <v>110.7</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>23</v>
@@ -1875,10 +1903,10 @@
         <v>40</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
+      </c>
+      <c r="F29" s="49" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1895,28 +1923,31 @@
         <v>40</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>135</v>
+        <v>136</v>
+      </c>
+      <c r="F30" s="49" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="44" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B31" s="45" t="s">
-        <v>139</v>
-      </c>
-      <c r="C31" s="46"/>
+        <v>137</v>
+      </c>
+      <c r="C31" s="50">
+        <f>0.27</f>
+        <v>0.27</v>
+      </c>
       <c r="D31" s="13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E31" s="13" t="s">
         <v>44</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1927,16 +1958,16 @@
         <v>38</v>
       </c>
       <c r="C32" s="14">
-        <v>0.27</v>
+        <v>11.2</v>
       </c>
       <c r="D32" s="13" t="s">
         <v>27</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2074,7 +2105,9 @@
       <c r="B40" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="C40" s="42"/>
+      <c r="C40" s="42">
+        <v>194000</v>
+      </c>
       <c r="D40" s="15" t="s">
         <v>40</v>
       </c>
@@ -2092,14 +2125,14 @@
       <c r="B41" s="41" t="s">
         <v>119</v>
       </c>
-      <c r="C41" s="16">
+      <c r="C41" s="42">
         <v>4520000</v>
       </c>
       <c r="D41" s="15" t="s">
         <v>40</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F41" s="40"/>
     </row>
@@ -2110,96 +2143,106 @@
       <c r="B42" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="C42" s="16">
-        <v>194000</v>
+      <c r="C42" s="46">
+        <v>66000</v>
       </c>
       <c r="D42" s="15" t="s">
         <v>40</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F42" s="16" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="43" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B43" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="C43" s="42"/>
+        <v>148</v>
+      </c>
+      <c r="C43" s="42">
+        <v>4520</v>
+      </c>
       <c r="D43" s="15" t="s">
         <v>43</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F43" s="16"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="43" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B44" s="24" t="s">
-        <v>151</v>
-      </c>
-      <c r="C44" s="42"/>
+        <v>149</v>
+      </c>
+      <c r="C44" s="42">
+        <v>3000</v>
+      </c>
       <c r="D44" s="15" t="s">
         <v>43</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F44" s="16"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="43" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B45" s="24" t="s">
-        <v>149</v>
-      </c>
-      <c r="C45" s="42"/>
+        <v>147</v>
+      </c>
+      <c r="C45" s="42">
+        <v>930000</v>
+      </c>
       <c r="D45" s="15" t="s">
         <v>43</v>
       </c>
       <c r="E45" s="15" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F45" s="16"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="43" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B46" s="24" t="s">
-        <v>153</v>
-      </c>
-      <c r="C46" s="42"/>
+        <v>151</v>
+      </c>
+      <c r="C46" s="42">
+        <v>890000</v>
+      </c>
       <c r="D46" s="15" t="s">
         <v>43</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F46" s="16"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="43" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B47" s="24" t="s">
-        <v>155</v>
-      </c>
-      <c r="C47" s="42"/>
+        <v>153</v>
+      </c>
+      <c r="C47" s="42">
+        <v>864000</v>
+      </c>
       <c r="D47" s="15" t="s">
         <v>43</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F47" s="16"/>
     </row>

</xml_diff>